<commit_message>
Change data input. Interpolate between high and low energy demand value for average number of occupants #19
</commit_message>
<xml_diff>
--- a/pycity_calc/data/BaseData/Specific_Demand_Data/Stromspiegel2017_spec_el_energy_demand.xlsx
+++ b/pycity_calc/data/BaseData/Specific_Demand_Data/Stromspiegel2017_spec_el_energy_demand.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pycity_calc\pycity_calc\data\BaseData\Specific_Demand_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pyCity_calc_github\pycity_calc\data\BaseData\Specific_Demand_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Number of persons</t>
   </si>
@@ -36,6 +36,15 @@
   </si>
   <si>
     <t>MFH</t>
+  </si>
+  <si>
+    <t>Ref:</t>
+  </si>
+  <si>
+    <t>https://www.mieterbund.de/index.php?eID=tx_nawsecuredl&amp;u=0&amp;g=0&amp;t=1496495412&amp;hash=624f834b069c77c42b4a96024b56a6944f10bce4&amp;file=fileadmin/pdf/Stromspiegel/Stromspiegel-2017_Tabellen.pdf</t>
+  </si>
+  <si>
+    <t>Kategorie C</t>
   </si>
 </sst>
 </file>
@@ -378,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,11 +419,11 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="D2">
         <f>C2/B2</f>
-        <v>2500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -425,11 +434,11 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>3200</v>
+        <v>3000</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D11" si="0">C3/B3</f>
-        <v>1600</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,11 +449,11 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>3900</v>
+        <v>3500</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>1166.6666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -455,11 +464,11 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>4200</v>
+        <v>3800</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1050</v>
+        <v>950</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -470,11 +479,11 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>5400</v>
+        <v>4800</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1080</v>
+        <v>960</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -485,11 +494,11 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -500,11 +509,11 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>2200</v>
+        <v>2000</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -515,11 +524,11 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>2800</v>
+        <v>2400</v>
       </c>
       <c r="D9" s="1">
         <f>C9/B9</f>
-        <v>933.33333333333337</v>
+        <v>800</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,11 +539,11 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>3200</v>
+        <v>2800</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>700</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,11 +554,24 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>